<commit_message>
added exported *.py files - Luke related
</commit_message>
<xml_diff>
--- a/report/pics/graphs_top10.xlsx
+++ b/report/pics/graphs_top10.xlsx
@@ -228,7 +228,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -243,7 +243,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>Sheet1!$L$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -298,27 +298,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$8</c:f>
+              <c:f>Sheet1!$L$3:$L$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.9786</c:v>
+                  <c:v>0.9652</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9501</c:v>
+                  <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8879</c:v>
+                  <c:v>0.8655</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9165</c:v>
+                  <c:v>0.8681</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.9154</c:v>
+                  <c:v>0.8749</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9126</c:v>
+                  <c:v>0.8909</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -329,7 +329,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$2</c:f>
+              <c:f>Sheet1!$P$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -384,27 +384,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$3:$H$8</c:f>
+              <c:f>Sheet1!$P$3:$P$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.8392</c:v>
+                  <c:v>0.7994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8432</c:v>
+                  <c:v>0.8019</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8575</c:v>
+                  <c:v>0.8257</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8832</c:v>
+                  <c:v>0.8446</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.895</c:v>
+                  <c:v>0.8622</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8967</c:v>
+                  <c:v>0.8588</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -415,7 +415,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$2</c:f>
+              <c:f>Sheet1!$M$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -470,27 +470,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$8</c:f>
+              <c:f>Sheet1!$M$3:$M$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.9501</c:v>
+                  <c:v>0.9372</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8086</c:v>
+                  <c:v>0.8954</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5763</c:v>
+                  <c:v>0.7147</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7371</c:v>
+                  <c:v>0.7128</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7445</c:v>
+                  <c:v>0.7343</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.7397</c:v>
+                  <c:v>0.7861</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -501,7 +501,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$2</c:f>
+              <c:f>Sheet1!$Q$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -556,27 +556,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$3:$I$8</c:f>
+              <c:f>Sheet1!$Q$3:$Q$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.532</c:v>
+                  <c:v>0.6141</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.3219</c:v>
+                  <c:v>0.4966</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4868</c:v>
+                  <c:v>0.6313</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6373</c:v>
+                  <c:v>0.6657</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.6874</c:v>
+                  <c:v>0.709</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.6957</c:v>
+                  <c:v>0.7233</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -584,11 +584,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="2821171"/>
-        <c:axId val="8696608"/>
+        <c:axId val="2700506"/>
+        <c:axId val="16665115"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2821171"/>
+        <c:axId val="2700506"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -623,14 +623,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8696608"/>
+        <c:crossAx val="16665115"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8696608"/>
+        <c:axId val="16665115"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -675,7 +675,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2821171"/>
+        <c:crossAx val="2700506"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -711,7 +711,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -726,7 +726,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$2</c:f>
+              <c:f>Sheet1!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -781,27 +781,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$3:$L$8</c:f>
+              <c:f>Sheet1!$D$3:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.9652</c:v>
+                  <c:v>0.9786</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.95</c:v>
+                  <c:v>0.9501</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8655</c:v>
+                  <c:v>0.8879</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8681</c:v>
+                  <c:v>0.9165</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.8749</c:v>
+                  <c:v>0.9154</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8909</c:v>
+                  <c:v>0.9126</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -812,7 +812,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$2</c:f>
+              <c:f>Sheet1!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -867,27 +867,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$3:$P$8</c:f>
+              <c:f>Sheet1!$H$3:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.7994</c:v>
+                  <c:v>0.8392</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8019</c:v>
+                  <c:v>0.8432</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8257</c:v>
+                  <c:v>0.8575</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8446</c:v>
+                  <c:v>0.8832</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.8622</c:v>
+                  <c:v>0.895</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8588</c:v>
+                  <c:v>0.8967</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -898,7 +898,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$2</c:f>
+              <c:f>Sheet1!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -953,27 +953,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$3:$M$8</c:f>
+              <c:f>Sheet1!$E$3:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.9372</c:v>
+                  <c:v>0.9501</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8954</c:v>
+                  <c:v>0.8086</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7147</c:v>
+                  <c:v>0.5763</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7128</c:v>
+                  <c:v>0.7371</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7343</c:v>
+                  <c:v>0.7445</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.7861</c:v>
+                  <c:v>0.7397</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -984,7 +984,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$2</c:f>
+              <c:f>Sheet1!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1039,27 +1039,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$3:$Q$8</c:f>
+              <c:f>Sheet1!$I$3:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.6141</c:v>
+                  <c:v>0.532</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4966</c:v>
+                  <c:v>0.3219</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6313</c:v>
+                  <c:v>0.4868</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6657</c:v>
+                  <c:v>0.6373</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.709</c:v>
+                  <c:v>0.6874</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.7233</c:v>
+                  <c:v>0.6957</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1067,11 +1067,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="89809652"/>
-        <c:axId val="15287104"/>
+        <c:axId val="42317118"/>
+        <c:axId val="5057582"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89809652"/>
+        <c:axId val="42317118"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1106,14 +1106,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15287104"/>
+        <c:crossAx val="5057582"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15287104"/>
+        <c:axId val="5057582"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1158,7 +1158,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89809652"/>
+        <c:crossAx val="42317118"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -1206,8 +1206,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>325800</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>145440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1216,7 +1216,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="119160" y="1491840"/>
-        <a:ext cx="5760000" cy="3241080"/>
+        <a:ext cx="5760000" cy="2880000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1236,8 +1236,8 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>165960</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>66600</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>30240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1246,7 +1246,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="6207840" y="1539360"/>
-        <a:ext cx="5760000" cy="3241440"/>
+        <a:ext cx="5760000" cy="2880000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">

</xml_diff>